<commit_message>
Updated dates in South collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/SOUTH COLLECTION.xlsx
+++ b/Photographic Archive/SOUTH COLLECTION.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -2815,9 +2818,9 @@
   </sheetPr>
   <dimension ref="A1:Z323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q9" sqref="Q9"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated collection data in South Collection
</commit_message>
<xml_diff>
--- a/Photographic Archive/SOUTH COLLECTION.xlsx
+++ b/Photographic Archive/SOUTH COLLECTION.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -2800,9 +2800,9 @@
   </sheetPr>
   <dimension ref="A1:Z322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2814,7 +2814,7 @@
     <col min="7" max="7" width="39.44140625" customWidth="1"/>
     <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.77734375" customWidth="1"/>
-    <col min="11" max="14" width="12.6640625" customWidth="1"/>
+    <col min="11" max="14" width="12.6640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>